<commit_message>
Book a class - session - group - individual
</commit_message>
<xml_diff>
--- a/Screenshots/Add class Report.xlsx
+++ b/Screenshots/Add class Report.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="101">
   <si>
     <t>key</t>
   </si>
@@ -250,6 +250,85 @@
   </si>
   <si>
     <t>Tutor add class submitted successfully :[Class added successfully.]</t>
+  </si>
+  <si>
+    <t>./Screenshots/2022-11-15-16-28-36.png</t>
+  </si>
+  <si>
+    <t>16/11/2022</t>
+  </si>
+  <si>
+    <t>D:\test\picturesprofile1\bharat3.jpg</t>
+  </si>
+  <si>
+    <t>./Screenshots/2022-11-15-16-33-29.png</t>
+  </si>
+  <si>
+    <t>./Screenshots/2022-11-15-16-35-30.png</t>
+  </si>
+  <si>
+    <t>Tutor add class has error : stale element reference: element is not attached to the page document
+  (Session info: chrome=107.0.5304.107)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/stale_element_reference.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:25:53'
+System info: host: 'LAPTOP-A5ODB7KC', ip: '192.168.137.1', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_282'
+Driver info: com.kms.katalon.selenium.driver.CChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 107.0.5304.107, chrome: {chromedriverVersion: 107.0.5304.62 (1eec40d3a576..., userDataDir: C:\Users\Srinivas\AppData\L...}, goog:chromeOptions: {debuggerAddress: localhost:60665}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: fd215f62ad7c00038f0515408271d41c</t>
+  </si>
+  <si>
+    <t>tutor54@nkt.com</t>
+  </si>
+  <si>
+    <t>Draw 2</t>
+  </si>
+  <si>
+    <t>Mudaliarpet</t>
+  </si>
+  <si>
+    <t>GHJ56GHJK58</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>mv class special 16/11 - 31/12</t>
+  </si>
+  <si>
+    <t>./Screenshots/2022-11-15-17-42-48.png</t>
+  </si>
+  <si>
+    <t>./Screenshots/2022-11-15-17-44-29.png</t>
+  </si>
+  <si>
+    <t>Oil Painting</t>
+  </si>
+  <si>
+    <t>friday</t>
+  </si>
+  <si>
+    <t>17/11/2022</t>
+  </si>
+  <si>
+    <t>sess class special 17/11 - 31/12</t>
+  </si>
+  <si>
+    <t>./Screenshots/2022-11-16-11-14-34.png</t>
+  </si>
+  <si>
+    <t>./Screenshots/2022-11-16-11-16-26.png</t>
+  </si>
+  <si>
+    <t>Tutor add class submission has error :[]</t>
+  </si>
+  <si>
+    <t>Oil Painting1</t>
+  </si>
+  <si>
+    <t>./Screenshots/2022-11-16-18-01-25.png</t>
+  </si>
+  <si>
+    <t>./Screenshots/2022-11-16-18-03-30.png</t>
   </si>
 </sst>
 </file>
@@ -257,7 +336,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -295,8 +374,62 @@
       <i val="true"/>
       <color indexed="12"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <i val="true"/>
+      <color indexed="12"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <i val="true"/>
+      <color indexed="12"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <i val="true"/>
+      <color indexed="12"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <i val="true"/>
+      <color indexed="12"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <i val="true"/>
+      <color indexed="12"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <i val="true"/>
+      <color indexed="12"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <i val="true"/>
+      <color indexed="12"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <i val="true"/>
+      <color indexed="12"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <i val="true"/>
+      <color indexed="12"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="26">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -331,6 +464,96 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
       </patternFill>
     </fill>
   </fills>
@@ -346,7 +569,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="28">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
     <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
@@ -355,8 +578,26 @@
     <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
     <xf applyFill="true" borderId="0" fillId="5" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="true" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf applyFill="true" borderId="0" fillId="7" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="11" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="13" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="15" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="17" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="19" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="21" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="23" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -637,7 +878,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AL5"/>
+  <dimension ref="A1:AL14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
@@ -659,7 +900,7 @@
     <col min="12" max="12" bestFit="true" customWidth="true" width="7.33984375" collapsed="true"/>
     <col min="13" max="13" bestFit="true" customWidth="true" width="18.2109375" collapsed="true"/>
     <col min="14" max="14" bestFit="true" customWidth="true" width="19.38671875" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="10.75390625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="12.1015625" collapsed="true"/>
     <col min="16" max="16" bestFit="true" customWidth="true" width="19.45703125" collapsed="true"/>
     <col min="17" max="17" bestFit="true" customWidth="true" width="14.8046875" collapsed="true"/>
     <col min="18" max="18" bestFit="true" customWidth="true" width="22.70703125" collapsed="true"/>
@@ -677,9 +918,9 @@
     <col min="30" max="30" bestFit="true" customWidth="true" width="61.3984375" collapsed="true"/>
     <col min="31" max="31" bestFit="true" customWidth="true" width="40.3671875" collapsed="true"/>
     <col min="32" max="32" bestFit="true" customWidth="true" width="7.109375" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="27.8828125" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="28.8046875" collapsed="true"/>
     <col min="35" max="35" bestFit="true" customWidth="true" width="40.25390625" collapsed="true"/>
-    <col min="36" max="36" bestFit="true" customWidth="true" width="59.75390625" collapsed="true"/>
+    <col min="36" max="36" bestFit="true" customWidth="true" width="255.0" collapsed="true"/>
     <col min="37" max="37" bestFit="true" customWidth="true" width="9.30078125" collapsed="true"/>
   </cols>
   <sheetData>
@@ -1223,14 +1464,1004 @@
       <c r="AG5" t="s">
         <v>65</v>
       </c>
-      <c r="AI5" t="s" s="9">
+      <c r="AI5" s="9" t="s">
         <v>75</v>
       </c>
       <c r="AJ5" t="s">
         <v>76</v>
       </c>
-      <c r="AK5" t="s" s="8">
+      <c r="AK5" s="8" t="s">
         <v>66</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6" t="s">
+        <v>73</v>
+      </c>
+      <c r="J6" t="s">
+        <v>44</v>
+      </c>
+      <c r="K6" t="s">
+        <v>45</v>
+      </c>
+      <c r="L6" t="s">
+        <v>46</v>
+      </c>
+      <c r="M6" t="s">
+        <v>47</v>
+      </c>
+      <c r="N6" t="s">
+        <v>48</v>
+      </c>
+      <c r="O6" t="s">
+        <v>49</v>
+      </c>
+      <c r="P6" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>51</v>
+      </c>
+      <c r="R6" t="s">
+        <v>52</v>
+      </c>
+      <c r="S6" t="s">
+        <v>53</v>
+      </c>
+      <c r="T6" t="s">
+        <v>41</v>
+      </c>
+      <c r="U6" t="s">
+        <v>54</v>
+      </c>
+      <c r="V6" t="s">
+        <v>41</v>
+      </c>
+      <c r="W6" t="s">
+        <v>55</v>
+      </c>
+      <c r="X6" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>65</v>
+      </c>
+      <c r="AI6" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>68</v>
+      </c>
+      <c r="AK6" s="10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I7" t="s">
+        <v>73</v>
+      </c>
+      <c r="J7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L7" t="s">
+        <v>46</v>
+      </c>
+      <c r="M7" t="s">
+        <v>47</v>
+      </c>
+      <c r="N7" t="s">
+        <v>48</v>
+      </c>
+      <c r="O7" t="s">
+        <v>49</v>
+      </c>
+      <c r="P7" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>51</v>
+      </c>
+      <c r="R7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S7" t="s">
+        <v>53</v>
+      </c>
+      <c r="T7" t="s">
+        <v>41</v>
+      </c>
+      <c r="U7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V7" t="s">
+        <v>41</v>
+      </c>
+      <c r="W7" t="s">
+        <v>55</v>
+      </c>
+      <c r="X7" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG7" t="s">
+        <v>65</v>
+      </c>
+      <c r="AI7" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="AJ7" t="s">
+        <v>68</v>
+      </c>
+      <c r="AK7" s="12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" t="s">
+        <v>42</v>
+      </c>
+      <c r="I8" t="s">
+        <v>73</v>
+      </c>
+      <c r="J8" t="s">
+        <v>44</v>
+      </c>
+      <c r="K8" t="s">
+        <v>45</v>
+      </c>
+      <c r="L8" t="s">
+        <v>46</v>
+      </c>
+      <c r="M8" t="s">
+        <v>47</v>
+      </c>
+      <c r="N8" t="s">
+        <v>48</v>
+      </c>
+      <c r="O8" t="s">
+        <v>49</v>
+      </c>
+      <c r="P8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>51</v>
+      </c>
+      <c r="R8" t="s">
+        <v>52</v>
+      </c>
+      <c r="S8" t="s">
+        <v>53</v>
+      </c>
+      <c r="T8" t="s">
+        <v>41</v>
+      </c>
+      <c r="U8" t="s">
+        <v>54</v>
+      </c>
+      <c r="V8" t="s">
+        <v>41</v>
+      </c>
+      <c r="W8" t="s">
+        <v>55</v>
+      </c>
+      <c r="X8" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG8" t="s">
+        <v>65</v>
+      </c>
+      <c r="AI8" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="AJ8" t="s">
+        <v>82</v>
+      </c>
+      <c r="AK8" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" t="s">
+        <v>83</v>
+      </c>
+      <c r="E9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H9" t="s">
+        <v>42</v>
+      </c>
+      <c r="I9" t="s">
+        <v>84</v>
+      </c>
+      <c r="J9" t="s">
+        <v>44</v>
+      </c>
+      <c r="K9" t="s">
+        <v>45</v>
+      </c>
+      <c r="L9" t="s">
+        <v>46</v>
+      </c>
+      <c r="M9" t="s">
+        <v>47</v>
+      </c>
+      <c r="N9" t="s">
+        <v>48</v>
+      </c>
+      <c r="O9" t="s">
+        <v>85</v>
+      </c>
+      <c r="P9" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>51</v>
+      </c>
+      <c r="R9" t="s">
+        <v>52</v>
+      </c>
+      <c r="S9" t="s">
+        <v>53</v>
+      </c>
+      <c r="T9" t="s">
+        <v>41</v>
+      </c>
+      <c r="U9" t="s">
+        <v>54</v>
+      </c>
+      <c r="V9" t="s">
+        <v>41</v>
+      </c>
+      <c r="W9" t="s">
+        <v>55</v>
+      </c>
+      <c r="X9" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>86</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>87</v>
+      </c>
+      <c r="AG9" t="s">
+        <v>88</v>
+      </c>
+      <c r="AI9" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="AJ9" t="s">
+        <v>68</v>
+      </c>
+      <c r="AK9" s="16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" t="s">
+        <v>41</v>
+      </c>
+      <c r="H10" t="s">
+        <v>42</v>
+      </c>
+      <c r="I10" t="s">
+        <v>84</v>
+      </c>
+      <c r="J10" t="s">
+        <v>44</v>
+      </c>
+      <c r="K10" t="s">
+        <v>45</v>
+      </c>
+      <c r="L10" t="s">
+        <v>46</v>
+      </c>
+      <c r="M10" t="s">
+        <v>47</v>
+      </c>
+      <c r="N10" t="s">
+        <v>48</v>
+      </c>
+      <c r="O10" t="s">
+        <v>85</v>
+      </c>
+      <c r="P10" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>51</v>
+      </c>
+      <c r="R10" t="s">
+        <v>52</v>
+      </c>
+      <c r="S10" t="s">
+        <v>53</v>
+      </c>
+      <c r="T10" t="s">
+        <v>41</v>
+      </c>
+      <c r="U10" t="s">
+        <v>54</v>
+      </c>
+      <c r="V10" t="s">
+        <v>41</v>
+      </c>
+      <c r="W10" t="s">
+        <v>55</v>
+      </c>
+      <c r="X10" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>86</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>87</v>
+      </c>
+      <c r="AG10" t="s">
+        <v>88</v>
+      </c>
+      <c r="AI10" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="AJ10" t="s">
+        <v>76</v>
+      </c>
+      <c r="AK10" s="18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" t="s">
+        <v>83</v>
+      </c>
+      <c r="E11" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" t="s">
+        <v>41</v>
+      </c>
+      <c r="H11" t="s">
+        <v>42</v>
+      </c>
+      <c r="I11" t="s">
+        <v>91</v>
+      </c>
+      <c r="J11" t="s">
+        <v>44</v>
+      </c>
+      <c r="K11" t="s">
+        <v>45</v>
+      </c>
+      <c r="L11" t="s">
+        <v>46</v>
+      </c>
+      <c r="M11" t="s">
+        <v>47</v>
+      </c>
+      <c r="N11" t="s">
+        <v>48</v>
+      </c>
+      <c r="O11" t="s">
+        <v>85</v>
+      </c>
+      <c r="P11" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>51</v>
+      </c>
+      <c r="R11" t="s">
+        <v>52</v>
+      </c>
+      <c r="S11" t="s">
+        <v>53</v>
+      </c>
+      <c r="T11" t="s">
+        <v>41</v>
+      </c>
+      <c r="U11" t="s">
+        <v>92</v>
+      </c>
+      <c r="V11" t="s">
+        <v>41</v>
+      </c>
+      <c r="W11" t="s">
+        <v>55</v>
+      </c>
+      <c r="X11" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>86</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>87</v>
+      </c>
+      <c r="AG11" t="s">
+        <v>94</v>
+      </c>
+      <c r="AI11" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="AJ11" t="s">
+        <v>68</v>
+      </c>
+      <c r="AK11" s="20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" t="s">
+        <v>83</v>
+      </c>
+      <c r="E12" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" t="s">
+        <v>42</v>
+      </c>
+      <c r="I12" t="s">
+        <v>91</v>
+      </c>
+      <c r="J12" t="s">
+        <v>44</v>
+      </c>
+      <c r="K12" t="s">
+        <v>45</v>
+      </c>
+      <c r="L12" t="s">
+        <v>46</v>
+      </c>
+      <c r="M12" t="s">
+        <v>47</v>
+      </c>
+      <c r="N12" t="s">
+        <v>48</v>
+      </c>
+      <c r="O12" t="s">
+        <v>85</v>
+      </c>
+      <c r="P12" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>51</v>
+      </c>
+      <c r="R12" t="s">
+        <v>52</v>
+      </c>
+      <c r="S12" t="s">
+        <v>53</v>
+      </c>
+      <c r="T12" t="s">
+        <v>41</v>
+      </c>
+      <c r="U12" t="s">
+        <v>92</v>
+      </c>
+      <c r="V12" t="s">
+        <v>41</v>
+      </c>
+      <c r="W12" t="s">
+        <v>55</v>
+      </c>
+      <c r="X12" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>86</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AG12" t="s">
+        <v>94</v>
+      </c>
+      <c r="AI12" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="AJ12" t="s">
+        <v>97</v>
+      </c>
+      <c r="AK12" s="22" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" t="s">
+        <v>83</v>
+      </c>
+      <c r="E13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13" t="s">
+        <v>41</v>
+      </c>
+      <c r="H13" t="s">
+        <v>42</v>
+      </c>
+      <c r="I13" t="s">
+        <v>98</v>
+      </c>
+      <c r="J13" t="s">
+        <v>44</v>
+      </c>
+      <c r="K13" t="s">
+        <v>45</v>
+      </c>
+      <c r="L13" t="s">
+        <v>46</v>
+      </c>
+      <c r="M13" t="s">
+        <v>47</v>
+      </c>
+      <c r="N13" t="s">
+        <v>48</v>
+      </c>
+      <c r="O13" t="s">
+        <v>85</v>
+      </c>
+      <c r="P13" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>51</v>
+      </c>
+      <c r="R13" t="s">
+        <v>52</v>
+      </c>
+      <c r="S13" t="s">
+        <v>53</v>
+      </c>
+      <c r="T13" t="s">
+        <v>41</v>
+      </c>
+      <c r="U13" t="s">
+        <v>92</v>
+      </c>
+      <c r="V13" t="s">
+        <v>41</v>
+      </c>
+      <c r="W13" t="s">
+        <v>55</v>
+      </c>
+      <c r="X13" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>86</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF13" t="s">
+        <v>87</v>
+      </c>
+      <c r="AG13" t="s">
+        <v>94</v>
+      </c>
+      <c r="AI13" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="AJ13" t="s">
+        <v>68</v>
+      </c>
+      <c r="AK13" s="24" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" t="s">
+        <v>83</v>
+      </c>
+      <c r="E14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" t="s">
+        <v>41</v>
+      </c>
+      <c r="G14" t="s">
+        <v>41</v>
+      </c>
+      <c r="H14" t="s">
+        <v>42</v>
+      </c>
+      <c r="I14" t="s">
+        <v>98</v>
+      </c>
+      <c r="J14" t="s">
+        <v>44</v>
+      </c>
+      <c r="K14" t="s">
+        <v>45</v>
+      </c>
+      <c r="L14" t="s">
+        <v>46</v>
+      </c>
+      <c r="M14" t="s">
+        <v>47</v>
+      </c>
+      <c r="N14" t="s">
+        <v>48</v>
+      </c>
+      <c r="O14" t="s">
+        <v>85</v>
+      </c>
+      <c r="P14" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>51</v>
+      </c>
+      <c r="R14" t="s">
+        <v>52</v>
+      </c>
+      <c r="S14" t="s">
+        <v>53</v>
+      </c>
+      <c r="T14" t="s">
+        <v>41</v>
+      </c>
+      <c r="U14" t="s">
+        <v>92</v>
+      </c>
+      <c r="V14" t="s">
+        <v>41</v>
+      </c>
+      <c r="W14" t="s">
+        <v>55</v>
+      </c>
+      <c r="X14" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>86</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF14" t="s">
+        <v>87</v>
+      </c>
+      <c r="AG14" t="s">
+        <v>94</v>
+      </c>
+      <c r="AI14" t="s" s="27">
+        <v>100</v>
+      </c>
+      <c r="AJ14" t="s">
+        <v>97</v>
+      </c>
+      <c r="AK14" t="s" s="26">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1238,7 +2469,16 @@
     <hyperlink r:id="rId1" ref="AI2"/>
     <hyperlink r:id="rId2" ref="AI3"/>
     <hyperlink r:id="rId3" ref="AI4"/>
-    <hyperlink ref="AI5" r:id="rId4"/>
+    <hyperlink r:id="rId4" ref="AI5"/>
+    <hyperlink r:id="rId5" ref="AI6"/>
+    <hyperlink r:id="rId6" ref="AI7"/>
+    <hyperlink r:id="rId7" ref="AI8"/>
+    <hyperlink r:id="rId8" ref="AI9"/>
+    <hyperlink r:id="rId9" ref="AI10"/>
+    <hyperlink r:id="rId10" ref="AI11"/>
+    <hyperlink r:id="rId11" ref="AI12"/>
+    <hyperlink r:id="rId12" ref="AI13"/>
+    <hyperlink ref="AI14" r:id="rId13"/>
   </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>